<commit_message>
Updated ASML, created Nvidia and Palo Alto Networks
</commit_message>
<xml_diff>
--- a/ASML DCF 10-25-22.xlsx
+++ b/ASML DCF 10-25-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D309ED-7694-0042-8ECE-4C03DE3E4875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C10BBA7-ECDC-AC44-9407-75ED598A3E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23500" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="135">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Shares Outstanding</t>
   </si>
   <si>
-    <t>Price Per Share</t>
-  </si>
-  <si>
     <t>Current Price</t>
   </si>
   <si>
@@ -435,6 +432,12 @@
   </si>
   <si>
     <t>Upside / Downside</t>
+  </si>
+  <si>
+    <t>Fair Value Per Share</t>
+  </si>
+  <si>
+    <t>Price to Earnings Ratio</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -754,6 +757,9 @@
     </xf>
     <xf numFmtId="9" fontId="15" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1073,10 +1079,10 @@
   <dimension ref="A1:AI112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X70" sqref="X70"/>
+      <selection pane="bottomRight" activeCell="AF29" sqref="AF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3492,7 +3498,7 @@
         <v>0.3054</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="20" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
@@ -3576,6 +3582,9 @@
       </c>
       <c r="AB28" s="12">
         <v>13.59</v>
+      </c>
+      <c r="AF28" s="20" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -3662,6 +3671,10 @@
       </c>
       <c r="AB29" s="12">
         <v>13.56</v>
+      </c>
+      <c r="AF29" s="53">
+        <f>AG51/AB25</f>
+        <v>33.961928889358035</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -10064,7 +10077,7 @@
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AB108" s="46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AC108" s="47">
         <f>AC106/AC107</f>
@@ -10073,7 +10086,7 @@
     </row>
     <row r="109" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="AB109" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC109" s="49">
         <v>486.01</v>
@@ -10085,7 +10098,7 @@
     </row>
     <row r="111" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="AB111" s="50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC111" s="51" t="str">
         <f>IF(AC108&gt;AC109, "BUY", "SELL")</f>
@@ -10094,7 +10107,7 @@
     </row>
     <row r="112" spans="1:32" ht="17" x14ac:dyDescent="0.2">
       <c r="AB112" s="50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC112" s="52">
         <f>(AC108/AC109)-1</f>

</xml_diff>